<commit_message>
hora de entrada y hora salida
</commit_message>
<xml_diff>
--- a/registros_excel/2024-01-26.xlsx
+++ b/registros_excel/2024-01-26.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,21 +466,31 @@
           <t>Hora</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Hora Entrada</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Hora Salida</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1015463003</t>
+          <t>15961357</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Leonardo Maje</t>
+          <t>Mauricio Sanchez</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Gerencial</t>
+          <t>Administrativa</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -490,7 +500,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10:7:38</t>
+          <t>23:37:13</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>23:37:13</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>23:37:13</t>
         </is>
       </c>
     </row>
@@ -502,7 +522,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Julian Largo</t>
+          <t>Angela Betancur</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -517,24 +537,34 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>10:7:41</t>
+          <t>23:38:7</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>23:38:07</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>23:38:07</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1054398414</t>
+          <t>12345</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Julian Largo</t>
+          <t>Adm</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Administrativa</t>
+          <t>Operaciones</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -544,24 +574,34 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>10:34:48</t>
+          <t>23:38:12</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>23:38:12</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>23:38:12</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1054398414</t>
+          <t>12345</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Julian Largo</t>
+          <t>Adm</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Administrativa</t>
+          <t>Operaciones</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -571,24 +611,34 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10:36:2</t>
+          <t>23:41:2</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>23:38:12</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>23:41:02</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1015463003</t>
+          <t>1054398414</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Leonardo Maje</t>
+          <t>Angela Betancur</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Gerencial</t>
+          <t>Administrativa</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -598,7 +648,17 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>10:36:5</t>
+          <t>23:41:4</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>23:38:07</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>23:41:04</t>
         </is>
       </c>
     </row>
@@ -625,19 +685,29 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>12:16:26</t>
+          <t>23:43:14</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>23:37:13</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>23:43:14</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>15961357</t>
+          <t>1054398414</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mauricio Sanchez</t>
+          <t>Angela Betancur</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -652,24 +722,34 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>13:8:35</t>
+          <t>23:43:18</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>23:38:07</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>23:43:18</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>15961357</t>
+          <t>12345</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mauricio Sanchez</t>
+          <t>Adm</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Administrativa</t>
+          <t>Operaciones</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -679,277 +759,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>13:9:48</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>15961357</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Mauricio Sanchez</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Administrativa</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2024-01-26</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>13:11:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>15961357</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Mauricio Sanchez</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Administrativa</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2024-01-26</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>13:13:6</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>1015463003</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Leonardo Maje</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Gerencial</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>2024-01-26</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>13:13:25</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>1015463003</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Leonardo Maje</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Gerencial</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2024-01-26</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>13:16:53</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1015463003</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Leonardo Maje</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Gerencial</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>2024-01-26</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>13:18:17</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>15961357</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Mauricio Sanchez</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Administrativa</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>2024-01-26</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>13:18:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>1054398414</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Julian Largo</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Administrativa</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>2024-01-26</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>13:18:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>1054398414</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Julian Largo</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Administrativa</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>2024-01-26</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>13:19:53</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>1054398414</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Julian Largo</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Administrativa</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2024-01-26</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>13:21:14</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>12345</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Adm</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Operaciones</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>2024-01-26</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>13:28:32</t>
+          <t>23:43:20</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>23:38:12</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>23:43:20</t>
         </is>
       </c>
     </row>

</xml_diff>